<commit_message>
prove su whisper, compute type diverso
</commit_message>
<xml_diff>
--- a/decider/qualtrics/COCOA.xlsx
+++ b/decider/qualtrics/COCOA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\FINAL\modules\decider\qualtrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15C5792-10AD-4BAE-9BED-9843A0B79B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E442A5-72A9-4E1A-839F-F4916E947BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{E87CDDA5-73A2-47A4-A5A0-5710167BB230}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{E87CDDA5-73A2-47A4-A5A0-5710167BB230}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
   <si>
     <t>Nome</t>
   </si>
@@ -231,6 +231,30 @@
   </si>
   <si>
     <t>Portato cibo da casa</t>
+  </si>
+  <si>
+    <t>Ion</t>
+  </si>
+  <si>
+    <t>Andrei</t>
+  </si>
+  <si>
+    <t>Loretta</t>
+  </si>
+  <si>
+    <t>Ballerini</t>
+  </si>
+  <si>
+    <t>Elena</t>
+  </si>
+  <si>
+    <t>Barboni</t>
+  </si>
+  <si>
+    <t>Tramezzino cotto e formaggio</t>
+  </si>
+  <si>
+    <t>Pasta al ragu bolognese</t>
   </si>
 </sst>
 </file>
@@ -317,7 +341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -340,11 +364,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -383,6 +418,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -742,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DC4545-8B2D-445E-8D66-48E537455D2D}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -891,12 +929,8 @@
       <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>25</v>
-      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
@@ -1052,12 +1086,8 @@
       <c r="E15" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>48</v>
-      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
@@ -1135,26 +1165,24 @@
       <c r="B19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="11">
         <v>218</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="G19" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="13" t="s">
+      <c r="E19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="C20" s="4">
         <v>219</v>
@@ -1162,22 +1190,34 @@
       <c r="D20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
+      <c r="A21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="C21" s="3">
         <v>220</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="C22" s="4">
         <v>221</v>
       </c>
@@ -1187,8 +1227,12 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
+      <c r="A23" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="C23" s="3">
         <v>222</v>
       </c>
@@ -1198,8 +1242,12 @@
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="C24" s="4">
         <v>223</v>
       </c>
@@ -1209,8 +1257,12 @@
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
+      <c r="A25" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="C25" s="3">
         <v>224</v>
       </c>
@@ -1220,8 +1272,12 @@
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="C26" s="4">
         <v>225</v>
       </c>

</xml_diff>